<commit_message>
Fixed xlsx cells, report renderers and delta per item.
</commit_message>
<xml_diff>
--- a/reports/requests/templates/xlsx/template.xlsx
+++ b/reports/requests/templates/xlsx/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\canuarb00\Desktop\Connectors\adobe-reports\reports\requests\templates\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D48D8C-C4F3-4714-A0CA-C89C5E52EC2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F2A36EF-AECC-451A-898A-9FC677E5CD69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -285,7 +285,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -592,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
-      <selection activeCell="AI7" sqref="AI7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -743,6 +743,7 @@
   </sheetData>
   <autoFilter ref="A1:AI1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Pull request #25: CAD-1633: Added new column for displaying assignee name
Merge in SITC/adobe-reports from ~KARLA.NUNEZ/adobe-reports-fork:CAD-1633-p1-generate-the-report-with-the-assignee-name to master

Squashed commit of the following:

commit 707eddd27d9767325c00b510160bb504698e18a6
Author: Karla Nunez <Karla.Nunez@ingrammicro.com>
Date:   Thu Apr 11 14:28:50 2024 +0200

    CAD-1633: Added new column for displaying assignee name
</commit_message>
<xml_diff>
--- a/reports/requests/templates/xlsx/template.xlsx
+++ b/reports/requests/templates/xlsx/template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\knunez00\Documents\Repositorios\adobe-reports-fork\reports\requests\templates\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE419E1D-DF04-4CBE-9E52-AF782D32A1F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{006FB9B2-6252-42B2-ABAB-4225FBA91753}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$AJ$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$AK$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -28,7 +28,7 @@
     <author>Anastasia Tsyrendorzhieva</author>
   </authors>
   <commentList>
-    <comment ref="Z1" authorId="0" shapeId="0" xr:uid="{EC890D59-8278-4FBC-94F4-B761B1396BB4}">
+    <comment ref="AA1" authorId="0" shapeId="0" xr:uid="{EC890D59-8278-4FBC-94F4-B761B1396BB4}">
       <text>
         <r>
           <rPr>
@@ -52,7 +52,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD1" authorId="0" shapeId="0" xr:uid="{3DC2AE38-9C54-4B3C-A703-DECE6ADB4B6B}">
+    <comment ref="AE1" authorId="0" shapeId="0" xr:uid="{3DC2AE38-9C54-4B3C-A703-DECE6ADB4B6B}">
       <text>
         <r>
           <rPr>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Request ID</t>
   </si>
@@ -210,6 +210,9 @@
   </si>
   <si>
     <t>Assignee ID</t>
+  </si>
+  <si>
+    <t>Assignee Name</t>
   </si>
 </sst>
 </file>
@@ -601,57 +604,57 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AQ1"/>
+  <dimension ref="A1:AR1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="18.42578125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="23.140625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" style="4" customWidth="1"/>
-    <col min="9" max="9" width="27.140625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="29.7109375" style="4" customWidth="1"/>
-    <col min="11" max="11" width="24.140625" style="4" customWidth="1"/>
-    <col min="12" max="12" width="20.85546875" style="4" customWidth="1"/>
-    <col min="13" max="13" width="17.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="8.7109375" style="4"/>
-    <col min="18" max="18" width="22.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="26.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="17.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="21.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="16.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="22.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="20.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="16" style="4" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="10.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="19.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="15.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="11.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="18.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="18.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="12.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="20.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="19.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="16.7109375" style="4" customWidth="1"/>
-    <col min="44" max="16384" width="8.7109375" style="4"/>
+    <col min="1" max="3" width="18.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="23.140625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" style="4" customWidth="1"/>
+    <col min="10" max="10" width="27.140625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="29.7109375" style="4" customWidth="1"/>
+    <col min="12" max="12" width="24.140625" style="4" customWidth="1"/>
+    <col min="13" max="13" width="20.85546875" style="4" customWidth="1"/>
+    <col min="14" max="14" width="17.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="8.7109375" style="4"/>
+    <col min="19" max="19" width="22.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="26.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="17.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="21.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="19.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="16.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="22.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="20.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="12.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="9" style="4" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="16" style="4" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="19.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="11.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="18.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="18.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="20.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="19.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="16.7109375" style="4" customWidth="1"/>
+    <col min="45" max="16384" width="8.7109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -659,131 +662,134 @@
         <v>42</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AH1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AL1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AM1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AN1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AN1" s="3" t="s">
+      <c r="AO1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AO1" s="3" t="s">
+      <c r="AP1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AP1" s="3" t="s">
+      <c r="AQ1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AQ1" s="3" t="s">
+      <c r="AR1" s="3" t="s">
         <v>41</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AJ1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:AK1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
Added support of Renew Type PRs and Information about applied Adobe Flex Discounts per order
</commit_message>
<xml_diff>
--- a/reports/requests/templates/xlsx/template.xlsx
+++ b/reports/requests/templates/xlsx/template.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\canuarb00\Desktop\Connectors\adobe-reports\reports\requests\templates\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/l.cuadrado/Library/CloudStorage/GoogleDrive-luis.cuadrado@cloudblue.com/My Drive/Documents/devprojects/mcps/adobe_reports/reports/requests/templates/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F2A36EF-AECC-451A-898A-9FC677E5CD69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D9A413B-0E24-BC49-B99C-E14BBD3A5759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="700" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$AI$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$AT$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -28,7 +28,7 @@
     <author>Anastasia Tsyrendorzhieva</author>
   </authors>
   <commentList>
-    <comment ref="Y1" authorId="0" shapeId="0" xr:uid="{EC890D59-8278-4FBC-94F4-B761B1396BB4}">
+    <comment ref="AH1" authorId="0" shapeId="0" xr:uid="{EC890D59-8278-4FBC-94F4-B761B1396BB4}">
       <text>
         <r>
           <rPr>
@@ -52,7 +52,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC1" authorId="0" shapeId="0" xr:uid="{3DC2AE38-9C54-4B3C-A703-DECE6ADB4B6B}">
+    <comment ref="AN1" authorId="0" shapeId="0" xr:uid="{3DC2AE38-9C54-4B3C-A703-DECE6ADB4B6B}">
       <text>
         <r>
           <rPr>
@@ -60,7 +60,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Anastasia Tsyrendorzhieva:</t>
         </r>
@@ -69,7 +69,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Subcription - Fullfilment - Request - Parameters -- can be different emails inside</t>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Request ID</t>
   </si>
@@ -186,13 +186,67 @@
   </si>
   <si>
     <t>Exported At</t>
+  </si>
+  <si>
+    <t>commitment</t>
+  </si>
+  <si>
+    <t>commitment start date</t>
+  </si>
+  <si>
+    <t>commitment end date</t>
+  </si>
+  <si>
+    <t>recommitment</t>
+  </si>
+  <si>
+    <t>recommitment start date</t>
+  </si>
+  <si>
+    <t>recommitment end date</t>
+  </si>
+  <si>
+    <t>external reference id</t>
+  </si>
+  <si>
+    <t>Assignee ID</t>
+  </si>
+  <si>
+    <t>Assignee Name</t>
+  </si>
+  <si>
+    <t>Adobe Renewal Date</t>
+  </si>
+  <si>
+    <t>Prorata (days)</t>
+  </si>
+  <si>
+    <t>Discounted MPN</t>
+  </si>
+  <si>
+    <t>Discounted Adobe Order Id</t>
+  </si>
+  <si>
+    <t>Adobe Discount Id</t>
+  </si>
+  <si>
+    <t>Adobe Discount Code</t>
+  </si>
+  <si>
+    <t>Discount Group Licenses</t>
+  </si>
+  <si>
+    <t>Discount Group Consumables</t>
+  </si>
+  <si>
+    <t>Unit of Measure</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -218,19 +272,6 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -285,7 +326,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -590,158 +631,222 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI1"/>
+  <dimension ref="A1:BA1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.54296875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="23.453125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="25.7265625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="17.7265625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="21.453125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="23.08984375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="12.90625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="27.1796875" style="4" customWidth="1"/>
-    <col min="9" max="9" width="29.6328125" style="4" customWidth="1"/>
-    <col min="10" max="10" width="24.08984375" style="4" customWidth="1"/>
-    <col min="11" max="11" width="20.81640625" style="4" customWidth="1"/>
-    <col min="12" max="12" width="17.7265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.81640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="8.7265625" style="4"/>
-    <col min="17" max="17" width="22.36328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="26.90625" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.08984375" style="4" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.81640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.7265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.08984375" style="4" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="17.1796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="21.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19.7265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="16.81640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="22.1796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="20.1796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.81640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="16" style="4" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="10.08984375" style="4" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="19.36328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="15.1796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="36" max="16384" width="8.7265625" style="4"/>
+    <col min="1" max="3" width="18.5" style="4" customWidth="1"/>
+    <col min="4" max="4" width="23.5" style="4" customWidth="1"/>
+    <col min="5" max="5" width="25.6640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="21.5" style="4" customWidth="1"/>
+    <col min="8" max="8" width="23.1640625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="27.1640625" style="4" customWidth="1"/>
+    <col min="11" max="13" width="29.6640625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="24.1640625" style="4" customWidth="1"/>
+    <col min="15" max="16" width="20.83203125" style="4" customWidth="1"/>
+    <col min="17" max="17" width="17.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="25" width="8.6640625" style="4"/>
+    <col min="26" max="26" width="22.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="26.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="14.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="17.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="21.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="19.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="19.6640625" style="4" customWidth="1"/>
+    <col min="36" max="36" width="16.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="16.83203125" style="4" customWidth="1"/>
+    <col min="38" max="38" width="16.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="22.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="20.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="9" style="4" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="16" style="4" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="10.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="19.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="15.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="11.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="18.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="18.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="12.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="20.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="19.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="16.6640625" style="4" customWidth="1"/>
+    <col min="54" max="16384" width="8.6640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:53" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="T1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AI1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AL1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AN1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AO1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AP1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AQ1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AR1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>34</v>
+      </c>
+      <c r="AU1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AV1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AW1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AX1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AY1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AZ1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="BA1" s="3" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AI1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:AT1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
Merged in feature/new-CBPFR-1726 (pull request #1)
Added support of Renew Type PRs and Information about applied Adobe Flex Discounts per order

* Added support of Renew Type PRs and Information about applied Adobe Flex Discounts per order


Approved-by: Juan Diego
Approved-by: Karla Nunez
Approved-by: Pablo Garcia de los Salmones
</commit_message>
<xml_diff>
--- a/reports/requests/templates/xlsx/template.xlsx
+++ b/reports/requests/templates/xlsx/template.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\luccao\adobe-reports\reports\requests\templates\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/l.cuadrado/Library/CloudStorage/GoogleDrive-luis.cuadrado@cloudblue.com/My Drive/Documents/devprojects/mcps/adobe-reports/reports/requests/templates/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FBAE2CD-89A1-454E-B596-1321B2DBD26F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E138DE4D-9F85-BC42-A808-6C359A163209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13840" yWindow="-11880" windowWidth="32280" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$AM$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$AP$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -28,7 +28,7 @@
     <author>Anastasia Tsyrendorzhieva</author>
   </authors>
   <commentList>
-    <comment ref="AA1" authorId="0" shapeId="0" xr:uid="{EC890D59-8278-4FBC-94F4-B761B1396BB4}">
+    <comment ref="AH1" authorId="0" shapeId="0" xr:uid="{EC890D59-8278-4FBC-94F4-B761B1396BB4}">
       <text>
         <r>
           <rPr>
@@ -52,7 +52,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AG1" authorId="0" shapeId="0" xr:uid="{3DC2AE38-9C54-4B3C-A703-DECE6ADB4B6B}">
+    <comment ref="AN1" authorId="0" shapeId="0" xr:uid="{3DC2AE38-9C54-4B3C-A703-DECE6ADB4B6B}">
       <text>
         <r>
           <rPr>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>Request ID</t>
   </si>
@@ -170,18 +170,6 @@
     <t>Adobe User Email</t>
   </si>
   <si>
-    <t>Currency</t>
-  </si>
-  <si>
-    <t>Cost</t>
-  </si>
-  <si>
-    <t>Reseller Cost</t>
-  </si>
-  <si>
-    <t>MSRP</t>
-  </si>
-  <si>
     <t>Connection Type</t>
   </si>
   <si>
@@ -219,6 +207,27 @@
   </si>
   <si>
     <t>Prorata (days)</t>
+  </si>
+  <si>
+    <t>Discount Group Licenses</t>
+  </si>
+  <si>
+    <t>Discount Group Consumables</t>
+  </si>
+  <si>
+    <t>Unit of Measure</t>
+  </si>
+  <si>
+    <t>Discounted MPN</t>
+  </si>
+  <si>
+    <t>Discounted Adobe Order Id</t>
+  </si>
+  <si>
+    <t>Adobe Discount Id</t>
+  </si>
+  <si>
+    <t>Adobe Discount Code</t>
   </si>
 </sst>
 </file>
@@ -610,68 +619,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AT1"/>
+  <dimension ref="A1:AW1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="AE5" sqref="AE5"/>
+    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
+      <selection activeCell="X1" sqref="X1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="18.42578125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="23.140625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" style="4" customWidth="1"/>
-    <col min="10" max="10" width="27.140625" style="4" customWidth="1"/>
-    <col min="11" max="11" width="29.7109375" style="4" customWidth="1"/>
-    <col min="12" max="12" width="24.140625" style="4" customWidth="1"/>
-    <col min="13" max="13" width="20.85546875" style="4" customWidth="1"/>
-    <col min="14" max="14" width="17.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="8.7109375" style="4"/>
-    <col min="19" max="19" width="22.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="26.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="17.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="21.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="19.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="19.7109375" style="4" customWidth="1"/>
-    <col min="29" max="29" width="16.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.85546875" style="4" customWidth="1"/>
-    <col min="31" max="31" width="16.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="22.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="20.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="16" style="4" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="10.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="19.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="15.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="11.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="18.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="18.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="12.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="20.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="19.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="16.7109375" style="4" customWidth="1"/>
-    <col min="47" max="16384" width="8.7109375" style="4"/>
+    <col min="1" max="3" width="18.5" style="4" customWidth="1"/>
+    <col min="4" max="4" width="23.5" style="4" customWidth="1"/>
+    <col min="5" max="5" width="25.6640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="21.5" style="4" customWidth="1"/>
+    <col min="8" max="8" width="23.1640625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="27.1640625" style="4" customWidth="1"/>
+    <col min="11" max="13" width="29.6640625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="24.1640625" style="4" customWidth="1"/>
+    <col min="15" max="16" width="20.83203125" style="4" customWidth="1"/>
+    <col min="17" max="17" width="17.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="25" width="8.6640625" style="4"/>
+    <col min="26" max="26" width="22.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="26.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="14.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="17.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="21.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="19.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="19.6640625" style="4" customWidth="1"/>
+    <col min="36" max="36" width="16.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="16.83203125" style="4" customWidth="1"/>
+    <col min="38" max="38" width="16.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="22.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="20.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="19.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="11.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="18.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="18.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="12.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="20.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="19.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="16.6640625" style="4" customWidth="1"/>
+    <col min="50" max="16384" width="8.6640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:49" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -698,113 +703,122 @@
         <v>8</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="T1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AB1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AI1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AD1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AL1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AN1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AO1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AP1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AQ1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AR1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AS1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AT1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AN1" s="3" t="s">
+      <c r="AU1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AO1" s="3" t="s">
+      <c r="AV1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AP1" s="3" t="s">
+      <c r="AW1" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="AQ1" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AR1" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="AS1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AT1" s="3" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AM1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:AP1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>